<commit_message>
Improved buttonHide2Clicked method. Added error traceback. Added template rightclick menu to MT housing table
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -580,17 +580,17 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
     </row>
@@ -745,17 +745,17 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
     </row>
@@ -910,17 +910,17 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
     </row>
@@ -1075,17 +1075,17 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
     </row>
@@ -1240,17 +1240,17 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
     </row>
@@ -1405,17 +1405,17 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
     </row>
@@ -1570,17 +1570,17 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
     </row>
@@ -1735,17 +1735,17 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>-1.0</t>
+          <t>-1</t>
         </is>
       </c>
     </row>
@@ -1856,6 +1856,116 @@
       <c r="K26" t="inlineStr">
         <is>
           <t>12906.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>TPS-Line</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>CR</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>TPS-Line</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>FL</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>410.0</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>413.2</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>406.8</t>
         </is>
       </c>
     </row>
@@ -2033,17 +2143,17 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>4860</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>4866</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>4854</t>
+          <t>-1</t>
         </is>
       </c>
     </row>
@@ -2475,17 +2585,17 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>4860</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>4866</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>4854</t>
+          <t>-1</t>
         </is>
       </c>
     </row>
@@ -3828,17 +3938,17 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>4860</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>4866</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>4854</t>
+          <t>-1</t>
         </is>
       </c>
     </row>

</xml_diff>